<commit_message>
Actualizado fecha. 5 de abril 12:10
</commit_message>
<xml_diff>
--- a/documentos.xlsx
+++ b/documentos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Id</t>
   </si>
@@ -29,28 +29,13 @@
     <t>Tipo de documento</t>
   </si>
   <si>
-    <t>nombre CCCC</t>
-  </si>
-  <si>
-    <t>usuario1</t>
-  </si>
-  <si>
-    <t>DOCUMENTO_CONTABLE</t>
-  </si>
-  <si>
-    <t>nombre FFFF</t>
-  </si>
-  <si>
-    <t>usuario2</t>
-  </si>
-  <si>
-    <t>DOCUMENTO_FACTURA</t>
-  </si>
-  <si>
     <t>nombre NNNN</t>
   </si>
   <si>
     <t>usuario3</t>
+  </si>
+  <si>
+    <t>Fri Apr 05 12:09:13 CEST 2019</t>
   </si>
   <si>
     <t>DOCUMENTO_NOMINA</t>
@@ -109,7 +94,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -142,48 +127,14 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="n">
-        <v>43560.50182708333</v>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="n">
-        <v>43560.501992129626</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="n">
-        <v>43560.5021249537</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5"/>
+    <row r="3"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Creación de nuevos métodos, para generar PDFs. Clase del 09/04/2019 (Periodo de alternancia - Aytos).
</commit_message>
<xml_diff>
--- a/documentos.xlsx
+++ b/documentos.xlsx
@@ -29,16 +29,16 @@
     <t>Tipo de documento</t>
   </si>
   <si>
-    <t>nombre NNNN</t>
+    <t>Documento contable nº. 1</t>
   </si>
   <si>
-    <t>usuario3</t>
+    <t>usuario1</t>
   </si>
   <si>
-    <t>Fri Apr 05 12:09:13 CEST 2019</t>
+    <t>Tue Apr 09 13:50:25 CEST 2019</t>
   </si>
   <si>
-    <t>DOCUMENTO_NOMINA</t>
+    <t>DOCUMENTO_CONTABLE</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Mapper. Clase 11 de abril.
</commit_message>
<xml_diff>
--- a/documentos.xlsx
+++ b/documentos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Id</t>
   </si>
@@ -27,18 +27,6 @@
   </si>
   <si>
     <t>Tipo de documento</t>
-  </si>
-  <si>
-    <t>Documento contable nº. 1</t>
-  </si>
-  <si>
-    <t>usuario1</t>
-  </si>
-  <si>
-    <t>Tue Apr 09 13:50:25 CEST 2019</t>
-  </si>
-  <si>
-    <t>DOCUMENTO_CONTABLE</t>
   </si>
 </sst>
 </file>
@@ -94,7 +82,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -117,24 +105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3"/>
+    <row r="2"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>